<commit_message>
changes to property logic in header
</commit_message>
<xml_diff>
--- a/rx_PSC_MerchandiseInventory.xlsx
+++ b/rx_PSC_MerchandiseInventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BerilP\repos\PSC-MerchandiseInventoryYSR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2CFB0E-F8F3-4072-A434-3381A855FBA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E39BD3A-CB39-45B4-BA3E-F0C5F6498C34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -116,7 +116,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -139,6 +139,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -148,18 +157,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -481,7 +490,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -492,45 +501,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
     </row>
     <row r="4" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>